<commit_message>
Fix something in ExamResultTemplate.xlsx file
</commit_message>
<xml_diff>
--- a/HCT_Client/ExamResultTemplate.xlsx
+++ b/HCT_Client/ExamResultTemplate.xlsx
@@ -224,6 +224,10 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -233,10 +237,6 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -259,19 +259,17 @@
   </sheetPr>
   <dimension ref="A1:I27"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A7" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E12" activeCellId="0" sqref="E12"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A4" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C10" activeCellId="0" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="8.81770833333333"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="8.27083333333333"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="12.125"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="8.59895833333333"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="10.140625"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="10.6041666666667"/>
-    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="8.81770833333333"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="8.48958333333333"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="12.5677083333333"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="8.81770833333333"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="10.4739583333333"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="10.9166666666667"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -308,7 +306,7 @@
       <c r="D4" s="1"/>
       <c r="E4" s="1"/>
     </row>
-    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="6" customFormat="false" ht="6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A6" s="3"/>
       <c r="B6" s="3"/>
       <c r="C6" s="3"/>
@@ -332,7 +330,7 @@
       <c r="H8" s="4"/>
       <c r="I8" s="4"/>
     </row>
-    <row r="9" customFormat="false" ht="25.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="9" customFormat="false" ht="21" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A9" s="5"/>
       <c r="B9" s="6"/>
       <c r="C9" s="6"/>
@@ -348,6 +346,7 @@
       <c r="E10" s="6"/>
       <c r="F10" s="6"/>
     </row>
+    <row r="11" customFormat="false" ht="40.2" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="12" customFormat="false" ht="28.2" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A12" s="7" t="s">
         <v>6</v>
@@ -355,11 +354,11 @@
       <c r="B12" s="7"/>
       <c r="C12" s="7"/>
       <c r="D12" s="7"/>
-      <c r="E12" s="7"/>
-      <c r="F12" s="7"/>
-      <c r="G12" s="7"/>
-      <c r="H12" s="7"/>
-      <c r="I12" s="7"/>
+      <c r="E12" s="8"/>
+      <c r="F12" s="8"/>
+      <c r="G12" s="8"/>
+      <c r="H12" s="8"/>
+      <c r="I12" s="8"/>
     </row>
     <row r="13" customFormat="false" ht="28.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A13" s="7" t="s">
@@ -381,11 +380,11 @@
       <c r="B14" s="7"/>
       <c r="C14" s="7"/>
       <c r="D14" s="7"/>
-      <c r="E14" s="7"/>
-      <c r="F14" s="7"/>
-      <c r="G14" s="7"/>
-      <c r="H14" s="7"/>
-      <c r="I14" s="7"/>
+      <c r="E14" s="8"/>
+      <c r="F14" s="8"/>
+      <c r="G14" s="8"/>
+      <c r="H14" s="8"/>
+      <c r="I14" s="8"/>
     </row>
     <row r="15" customFormat="false" ht="28.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A15" s="7" t="s">
@@ -477,38 +476,38 @@
       <c r="I22" s="3"/>
     </row>
     <row r="25" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B25" s="8" t="s">
+      <c r="B25" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="C25" s="8"/>
-      <c r="D25" s="8"/>
-      <c r="E25" s="9"/>
-      <c r="F25" s="8" t="s">
+      <c r="C25" s="9"/>
+      <c r="D25" s="9"/>
+      <c r="E25" s="10"/>
+      <c r="F25" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="G25" s="8"/>
-      <c r="H25" s="8"/>
+      <c r="G25" s="9"/>
+      <c r="H25" s="9"/>
     </row>
     <row r="26" customFormat="false" ht="30.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B26" s="8" t="s">
+      <c r="B26" s="9" t="s">
         <v>16</v>
       </c>
-      <c r="C26" s="8"/>
-      <c r="D26" s="8"/>
-      <c r="E26" s="8"/>
-      <c r="F26" s="8" t="s">
+      <c r="C26" s="9"/>
+      <c r="D26" s="9"/>
+      <c r="E26" s="9"/>
+      <c r="F26" s="9" t="s">
         <v>16</v>
       </c>
-      <c r="G26" s="8"/>
-      <c r="H26" s="8"/>
+      <c r="G26" s="9"/>
+      <c r="H26" s="9"/>
     </row>
     <row r="27" customFormat="false" ht="26.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B27" s="10" t="s">
+      <c r="B27" s="11" t="s">
         <v>17</v>
       </c>
-      <c r="C27" s="10"/>
-      <c r="D27" s="10"/>
-      <c r="E27" s="8"/>
+      <c r="C27" s="11"/>
+      <c r="D27" s="11"/>
+      <c r="E27" s="9"/>
       <c r="F27" s="11" t="s">
         <v>18</v>
       </c>
@@ -516,8 +515,10 @@
       <c r="H27" s="11"/>
     </row>
   </sheetData>
-  <mergeCells count="7">
+  <mergeCells count="9">
     <mergeCell ref="A8:I8"/>
+    <mergeCell ref="E12:I12"/>
+    <mergeCell ref="E14:I14"/>
     <mergeCell ref="B25:D25"/>
     <mergeCell ref="F25:H25"/>
     <mergeCell ref="B26:D26"/>

</xml_diff>